<commit_message>
Working on the thesis and debuging ransac
</commit_message>
<xml_diff>
--- a/Code/iris detection/results/LPW_2_4.xlsx
+++ b/Code/iris detection/results/LPW_2_4.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>frame number</t>
   </si>
@@ -40,7 +40,13 @@
     <t>(412, 241)</t>
   </si>
   <si>
-    <t>(418, 251)</t>
+    <t>(409, 233)</t>
+  </si>
+  <si>
+    <t>(419, 250)</t>
+  </si>
+  <si>
+    <t>(414, 239)</t>
   </si>
 </sst>
 </file>
@@ -398,7 +404,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -435,19 +441,42 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
       </c>
       <c r="E2">
-        <v>11.6619037896906</v>
+        <v>11.40175425099138</v>
       </c>
       <c r="F2">
+        <v>7</v>
+      </c>
+      <c r="G2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>7.810249675906654</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+      <c r="G3">
         <v>6</v>
-      </c>
-      <c r="G2">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>